<commit_message>
Use case sensitive GEOM
</commit_message>
<xml_diff>
--- a/combined_data.xlsx
+++ b/combined_data.xlsx
@@ -22,9 +22,12 @@
     <sheet name="processed" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="ready_25978" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="ready_28582" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="processed1" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="ready_259781" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="ready_285821" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId17"/>
+    <externalReference r:id="rId20"/>
   </externalReferences>
   <definedNames>
     <definedName name="Crops">[1]Units!$A$2:$A$34</definedName>
@@ -2066,6 +2069,783 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ready_259781</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ready_285821</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" customHeight="1" defaultRowHeight="25"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="10" width="24.1640625"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="10" width="24.5"/>
+    <col customWidth="1" max="16384" min="3" style="10" width="10.83203125"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" customHeight="1" ht="25" r="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="2" s="2">
+      <c r="A2" s="10" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2" s="11" t="inlineStr">
+        <is>
+          <t>dpollard@ecotrust.org</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="3" s="2">
+      <c r="A3" s="10" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B3" s="11" t="inlineStr">
+        <is>
+          <t>25978</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="4" s="2">
+      <c r="A4" s="10" t="inlineStr">
+        <is>
+          <t>CRP</t>
+        </is>
+      </c>
+      <c r="B4" s="9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="5" s="2">
+      <c r="A5" s="10" t="inlineStr">
+        <is>
+          <t>CRPType</t>
+        </is>
+      </c>
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="6" s="2">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>GEOM</t>
+        </is>
+      </c>
+      <c r="B6" s="10" t="inlineStr">
+        <is>
+          <t>Polygon((-1575773.82987 270588.290829,-1576104.82596 270623.520321,-1576269.41581 270662.71954,-1576459.34745 270740.737118,-1576847.20878 270844.814266,-1576659.70878 271556.508602,-1575994.7576 271381.327938,-1576000.58768 271233.950008,-1575912.52128 271230.46368,-1575738.17557 271322.71954,-1575669.41581 271221.308407,-1575728.24393 271172.71954,-1575848.12675 271116.147274,-1575851.81815 271022.763485,-1575734.60135 270914.159969,-1575726.98417 270721.928524,-1575773.82987 270588.290829,-1575803.82987 270738.290829,-1575824.36698 270810.112118,-1575877.15995 270759.252743,-1575803.82987 270738.290829))</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="7" s="2">
+      <c r="A7" s="10" t="inlineStr">
+        <is>
+          <t>SRID</t>
+        </is>
+      </c>
+      <c r="B7" s="10" t="inlineStr">
+        <is>
+          <t>4326</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="8" s="2">
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>AREA</t>
+        </is>
+      </c>
+      <c r="B8" s="10" t="inlineStr">
+        <is>
+          <t>183</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="9" s="2">
+      <c r="A9" s="10" t="inlineStr">
+        <is>
+          <t>pre_80</t>
+        </is>
+      </c>
+      <c r="B9" s="10" t="inlineStr">
+        <is>
+          <t>Irrigation (Pre 1980s)</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="10" s="2">
+      <c r="A10" s="10" t="inlineStr">
+        <is>
+          <t>yr80_2000</t>
+        </is>
+      </c>
+      <c r="B10" s="10" t="inlineStr">
+        <is>
+          <t>Irrigated: Annual Crops in Rotation</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="11" s="2">
+      <c r="A11" s="10" t="inlineStr">
+        <is>
+          <t>till80_200</t>
+        </is>
+      </c>
+      <c r="B11" s="10" t="inlineStr">
+        <is>
+          <t>Intensive Tillage</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="12" s="2">
+      <c r="A12" s="10" t="inlineStr">
+        <is>
+          <t>crop_scenario_name</t>
+        </is>
+      </c>
+      <c r="B12" s="12" t="inlineStr">
+        <is>
+          <t>Todo_polygon_id25978Todo_scenario_id</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="13" s="2">
+      <c r="A13" s="10" t="inlineStr">
+        <is>
+          <t>YEAR</t>
+        </is>
+      </c>
+      <c r="B13" s="12" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="14" s="2">
+      <c r="A14" s="10" t="inlineStr">
+        <is>
+          <t>CROP_NUMBER</t>
+        </is>
+      </c>
+      <c r="B14" s="12" t="inlineStr">
+        <is>
+          <t>"1"</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="15" s="2">
+      <c r="A15" s="10" t="inlineStr">
+        <is>
+          <t>Ccop_name</t>
+        </is>
+      </c>
+      <c r="B15" s="10" t="inlineStr">
+        <is>
+          <t>Spring Wheat</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="16" s="2">
+      <c r="A16" s="10" t="inlineStr">
+        <is>
+          <t>planting_date</t>
+        </is>
+      </c>
+      <c r="B16" s="12" t="inlineStr">
+        <is>
+          <t>"01/01/1999"</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="17" s="2">
+      <c r="A17" s="10" t="inlineStr">
+        <is>
+          <t>continue_from_previous_year</t>
+        </is>
+      </c>
+      <c r="B17" s="13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="18" s="2">
+      <c r="A18" s="10" t="inlineStr">
+        <is>
+          <t>harvest_date</t>
+        </is>
+      </c>
+      <c r="B18" s="12" t="inlineStr">
+        <is>
+          <t>"01/01/1999"</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="19" s="2">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>grain</t>
+        </is>
+      </c>
+      <c r="B19" s="13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="20" s="2">
+      <c r="A20" s="10" t="inlineStr">
+        <is>
+          <t>yield</t>
+        </is>
+      </c>
+      <c r="B20" s="12" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="21" s="2">
+      <c r="A21" s="10" t="inlineStr">
+        <is>
+          <t>straw_stover_hay_removal</t>
+        </is>
+      </c>
+      <c r="B21" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="22" s="2">
+      <c r="A22" s="10" t="inlineStr">
+        <is>
+          <t>tillage_date</t>
+        </is>
+      </c>
+      <c r="B22" s="12" t="inlineStr">
+        <is>
+          <t>"01/01/1999"</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="23" s="2">
+      <c r="A23" s="10" t="inlineStr">
+        <is>
+          <t>tillage_type</t>
+        </is>
+      </c>
+      <c r="B23" s="12" t="inlineStr">
+        <is>
+          <t>Reduced Tillage</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="24" s="2">
+      <c r="A24" s="10" t="inlineStr">
+        <is>
+          <t>n_application_date</t>
+        </is>
+      </c>
+      <c r="B24" s="12" t="inlineStr">
+        <is>
+          <t>"01/01/1999"</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="25" s="2">
+      <c r="A25" s="10" t="inlineStr">
+        <is>
+          <t>n_application_type</t>
+        </is>
+      </c>
+      <c r="B25" s="12" t="inlineStr">
+        <is>
+          <t>Ammonium Nitrate</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="26" s="2">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>n_application_amount</t>
+        </is>
+      </c>
+      <c r="B26" s="12" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="27" s="2">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>n_application_method</t>
+        </is>
+      </c>
+      <c r="B27" s="12" t="inlineStr">
+        <is>
+          <t>Surface Broadcast</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="28" s="2">
+      <c r="A28" s="10" t="inlineStr">
+        <is>
+          <t>eep</t>
+        </is>
+      </c>
+      <c r="B28" s="12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="29" s="2">
+      <c r="A29" s="10" t="inlineStr">
+        <is>
+          <t>did_you_burn_residue</t>
+        </is>
+      </c>
+      <c r="B29" s="13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" customHeight="1" defaultRowHeight="25"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="10" width="24.1640625"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="10" width="24.5"/>
+    <col customWidth="1" max="16384" min="3" style="10" width="10.83203125"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" customHeight="1" ht="25" r="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="2" s="2">
+      <c r="A2" s="10" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2" s="11" t="inlineStr">
+        <is>
+          <t>dpollard@ecotrust.org</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="3" s="2">
+      <c r="A3" s="10" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B3" s="11" t="inlineStr">
+        <is>
+          <t>28582</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="4" s="2">
+      <c r="A4" s="10" t="inlineStr">
+        <is>
+          <t>CRP</t>
+        </is>
+      </c>
+      <c r="B4" s="9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="5" s="2">
+      <c r="A5" s="10" t="inlineStr">
+        <is>
+          <t>CRPType</t>
+        </is>
+      </c>
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="6" s="2">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>GEOM</t>
+        </is>
+      </c>
+      <c r="B6" s="10" t="inlineStr">
+        <is>
+          <t>Polygon((-1582013.82987 267048.290829,-1582003.54667 267084.867977,-1581977.26737 267058.559383,-1582013.82987 267048.290829,-1582013.82987 267048.290829,-1582054.96268 266837.631649,-1582190.31425 266382.460751,-1582454.60135 266434.067196,-1582717.92167 266524.184383,-1584455.22635 267032.514462,-1584563.21464 267067.568173,-1584333.61503 267934.067196,-1584127.5701 268664.584774,-1583705.22635 268504.741024,-1583482.98026 268500.214657,-1583238.99589 268559.687313,-1583108.5369 268622.99786,-1583003.71268 268676.992001,-1582716.25175 268775.385555,-1582508.82987 268771.152157,-1582273.63456 268775.942196,-1582091.55448 268656.572079,-1581979.17167 268490.795712,-1581912.16971 267572.441219,-1581907.98026 267367.099423,-1581939.09354 267271.283993,-1581999.12284 267213.583798,-1582028.5369 267152.99786,-1582059.73807 267092.397274,-1582013.82987 267048.290829))</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="7" s="2">
+      <c r="A7" s="10" t="inlineStr">
+        <is>
+          <t>SRID</t>
+        </is>
+      </c>
+      <c r="B7" s="10" t="inlineStr">
+        <is>
+          <t>4326</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="8" s="2">
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>AREA</t>
+        </is>
+      </c>
+      <c r="B8" s="10" t="inlineStr">
+        <is>
+          <t>1156</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="9" s="2">
+      <c r="A9" s="10" t="inlineStr">
+        <is>
+          <t>pre_80</t>
+        </is>
+      </c>
+      <c r="B9" s="10" t="inlineStr">
+        <is>
+          <t>Irrigation (Pre 1980s)</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="10" s="2">
+      <c r="A10" s="10" t="inlineStr">
+        <is>
+          <t>yr80_2000</t>
+        </is>
+      </c>
+      <c r="B10" s="10" t="inlineStr">
+        <is>
+          <t>Irrigated: Annual Crops in Rotation</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="11" s="2">
+      <c r="A11" s="10" t="inlineStr">
+        <is>
+          <t>till80_200</t>
+        </is>
+      </c>
+      <c r="B11" s="10" t="inlineStr">
+        <is>
+          <t>Intensive Tillage</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="12" s="2">
+      <c r="A12" s="10" t="inlineStr">
+        <is>
+          <t>crop_scenario_name</t>
+        </is>
+      </c>
+      <c r="B12" s="12" t="inlineStr">
+        <is>
+          <t>Todo_polygon_id28582Todo_scenario_id</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="13" s="2">
+      <c r="A13" s="10" t="inlineStr">
+        <is>
+          <t>YEAR</t>
+        </is>
+      </c>
+      <c r="B13" s="12" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="14" s="2">
+      <c r="A14" s="10" t="inlineStr">
+        <is>
+          <t>CROP_NUMBER</t>
+        </is>
+      </c>
+      <c r="B14" s="12" t="inlineStr">
+        <is>
+          <t>"1"</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="15" s="2">
+      <c r="A15" s="10" t="inlineStr">
+        <is>
+          <t>Ccop_name</t>
+        </is>
+      </c>
+      <c r="B15" s="10" t="inlineStr">
+        <is>
+          <t>Winter Wheat</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="16" s="2">
+      <c r="A16" s="10" t="inlineStr">
+        <is>
+          <t>planting_date</t>
+        </is>
+      </c>
+      <c r="B16" s="12" t="inlineStr">
+        <is>
+          <t>"01/01/1999"</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="17" s="2">
+      <c r="A17" s="10" t="inlineStr">
+        <is>
+          <t>continue_from_previous_year</t>
+        </is>
+      </c>
+      <c r="B17" s="13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="18" s="2">
+      <c r="A18" s="10" t="inlineStr">
+        <is>
+          <t>harvest_date</t>
+        </is>
+      </c>
+      <c r="B18" s="12" t="inlineStr">
+        <is>
+          <t>"01/01/1999"</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="19" s="2">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>grain</t>
+        </is>
+      </c>
+      <c r="B19" s="13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="20" s="2">
+      <c r="A20" s="10" t="inlineStr">
+        <is>
+          <t>yield</t>
+        </is>
+      </c>
+      <c r="B20" s="12" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="21" s="2">
+      <c r="A21" s="10" t="inlineStr">
+        <is>
+          <t>straw_stover_hay_removal</t>
+        </is>
+      </c>
+      <c r="B21" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="22" s="2">
+      <c r="A22" s="10" t="inlineStr">
+        <is>
+          <t>tillage_date</t>
+        </is>
+      </c>
+      <c r="B22" s="12" t="inlineStr">
+        <is>
+          <t>"01/01/1999"</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="23" s="2">
+      <c r="A23" s="10" t="inlineStr">
+        <is>
+          <t>tillage_type</t>
+        </is>
+      </c>
+      <c r="B23" s="12" t="inlineStr">
+        <is>
+          <t>Reduced Tillage</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="24" s="2">
+      <c r="A24" s="10" t="inlineStr">
+        <is>
+          <t>n_application_date</t>
+        </is>
+      </c>
+      <c r="B24" s="12" t="inlineStr">
+        <is>
+          <t>"01/01/1999"</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="25" s="2">
+      <c r="A25" s="10" t="inlineStr">
+        <is>
+          <t>n_application_type</t>
+        </is>
+      </c>
+      <c r="B25" s="12" t="inlineStr">
+        <is>
+          <t>Ammonium Nitrate</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="26" s="2">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>n_application_amount</t>
+        </is>
+      </c>
+      <c r="B26" s="12" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="27" s="2">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>n_application_method</t>
+        </is>
+      </c>
+      <c r="B27" s="12" t="inlineStr">
+        <is>
+          <t>Surface Broadcast</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="28" s="2">
+      <c r="A28" s="10" t="inlineStr">
+        <is>
+          <t>eep</t>
+        </is>
+      </c>
+      <c r="B28" s="12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="29" s="2">
+      <c r="A29" s="10" t="inlineStr">
+        <is>
+          <t>did_you_burn_residue</t>
+        </is>
+      </c>
+      <c r="B29" s="13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Next year harvest date for cover crops
</commit_message>
<xml_diff>
--- a/combined_data.xlsx
+++ b/combined_data.xlsx
@@ -5757,7 +5757,7 @@
       </c>
       <c r="F22" s="41" t="inlineStr">
         <is>
-          <t>04/07/2000</t>
+          <t>04/07/2001</t>
         </is>
       </c>
       <c r="G22" s="36" t="n">
@@ -5881,7 +5881,7 @@
       </c>
       <c r="F24" s="41" t="inlineStr">
         <is>
-          <t>04/07/2001</t>
+          <t>04/07/2002</t>
         </is>
       </c>
       <c r="G24" s="36" t="n">
@@ -6005,7 +6005,7 @@
       </c>
       <c r="F26" s="41" t="inlineStr">
         <is>
-          <t>04/07/2002</t>
+          <t>04/07/2003</t>
         </is>
       </c>
       <c r="G26" s="36" t="n">
@@ -6129,7 +6129,7 @@
       </c>
       <c r="F28" s="41" t="inlineStr">
         <is>
-          <t>04/08/2003</t>
+          <t>04/08/2004</t>
         </is>
       </c>
       <c r="G28" s="36" t="n">
@@ -6249,7 +6249,7 @@
       </c>
       <c r="F30" s="41" t="inlineStr">
         <is>
-          <t>04/07/2004</t>
+          <t>04/07/2005</t>
         </is>
       </c>
       <c r="G30" s="36" t="n">
@@ -6371,7 +6371,7 @@
       </c>
       <c r="F32" s="41" t="inlineStr">
         <is>
-          <t>04/07/2005</t>
+          <t>04/07/2006</t>
         </is>
       </c>
       <c r="G32" s="36" t="n">
@@ -6491,7 +6491,7 @@
       </c>
       <c r="F34" s="41" t="inlineStr">
         <is>
-          <t>04/07/2006</t>
+          <t>04/07/2007</t>
         </is>
       </c>
       <c r="G34" s="36" t="n">
@@ -6613,7 +6613,7 @@
       </c>
       <c r="F36" s="41" t="inlineStr">
         <is>
-          <t>04/08/2007</t>
+          <t>04/08/2008</t>
         </is>
       </c>
       <c r="G36" s="36" t="n">
@@ -6733,7 +6733,7 @@
       </c>
       <c r="F38" s="41" t="inlineStr">
         <is>
-          <t>04/07/2008</t>
+          <t>04/07/2009</t>
         </is>
       </c>
       <c r="G38" s="36" t="n">
@@ -6855,7 +6855,7 @@
       </c>
       <c r="F40" s="41" t="inlineStr">
         <is>
-          <t>04/07/2009</t>
+          <t>04/07/2010</t>
         </is>
       </c>
       <c r="G40" s="36" t="n">
@@ -6975,7 +6975,7 @@
       </c>
       <c r="F42" s="41" t="inlineStr">
         <is>
-          <t>04/07/2010</t>
+          <t>04/07/2011</t>
         </is>
       </c>
       <c r="G42" s="36" t="n">
@@ -7097,7 +7097,7 @@
       </c>
       <c r="F44" s="41" t="inlineStr">
         <is>
-          <t>04/08/2011</t>
+          <t>04/08/2012</t>
         </is>
       </c>
       <c r="G44" s="36" t="n">
@@ -7217,7 +7217,7 @@
       </c>
       <c r="F46" s="41" t="inlineStr">
         <is>
-          <t>04/07/2012</t>
+          <t>04/07/2013</t>
         </is>
       </c>
       <c r="G46" s="36" t="n">
@@ -7339,7 +7339,7 @@
       </c>
       <c r="F48" s="41" t="inlineStr">
         <is>
-          <t>04/07/2013</t>
+          <t>04/07/2014</t>
         </is>
       </c>
       <c r="G48" s="36" t="n">
@@ -7459,7 +7459,7 @@
       </c>
       <c r="F50" s="41" t="inlineStr">
         <is>
-          <t>04/07/2014</t>
+          <t>04/07/2015</t>
         </is>
       </c>
       <c r="G50" s="36" t="n">
@@ -7581,7 +7581,7 @@
       </c>
       <c r="F52" s="41" t="inlineStr">
         <is>
-          <t>04/08/2015</t>
+          <t>04/08/2016</t>
         </is>
       </c>
       <c r="G52" s="36" t="n">
@@ -7701,7 +7701,7 @@
       </c>
       <c r="F54" s="41" t="inlineStr">
         <is>
-          <t>04/07/2016</t>
+          <t>04/07/2017</t>
         </is>
       </c>
       <c r="G54" s="36" t="n">
@@ -7823,7 +7823,7 @@
       </c>
       <c r="F56" s="41" t="inlineStr">
         <is>
-          <t>04/07/2017</t>
+          <t>04/07/2018</t>
         </is>
       </c>
       <c r="G56" s="36" t="n">
@@ -7945,7 +7945,7 @@
       </c>
       <c r="F58" s="41" t="inlineStr">
         <is>
-          <t>04/07/2018</t>
+          <t>04/07/2019</t>
         </is>
       </c>
       <c r="G58" s="36" t="n">
@@ -8069,7 +8069,7 @@
       </c>
       <c r="F60" s="41" t="inlineStr">
         <is>
-          <t>04/07/2019</t>
+          <t>04/07/2020</t>
         </is>
       </c>
       <c r="G60" s="36" t="n">

</xml_diff>